<commit_message>
Rename TableFuncionarioDevicesView to Func...DevicesView and updating/fixing layouts
</commit_message>
<xml_diff>
--- a/Sistema de Gestao de Assiduidade/forms.xlsx
+++ b/Sistema de Gestao de Assiduidade/forms.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="80">
   <si>
     <t>FormName</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Alterar Dados do Funcionario</t>
   </si>
   <si>
-    <t>TableFuncionarioDeviceView</t>
-  </si>
-  <si>
     <t>DeviceDataUpdateView</t>
   </si>
   <si>
@@ -247,6 +244,18 @@
   </si>
   <si>
     <t>MDI Child</t>
+  </si>
+  <si>
+    <t>Bad Resize</t>
+  </si>
+  <si>
+    <t>MDI Child or Dialog</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>FuncionarioDeviceView</t>
   </si>
 </sst>
 </file>
@@ -270,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,6 +295,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -387,6 +402,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -696,7 +717,8 @@
     <col min="5" max="5" width="11.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1"/>
     <col min="7" max="7" width="17.75" style="1" customWidth="1"/>
-    <col min="8" max="10" width="9" style="1"/>
+    <col min="8" max="8" width="16.875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -719,7 +741,7 @@
         <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="11" customFormat="1" ht="15.75" thickBot="1">
@@ -736,7 +758,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -756,7 +778,7 @@
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -776,7 +798,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -796,7 +818,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -813,7 +835,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1">
@@ -827,7 +849,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" ht="15.75" thickBot="1">
@@ -844,7 +866,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -864,7 +886,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -881,7 +903,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1">
@@ -895,7 +917,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="7" customFormat="1" ht="15.75" thickBot="1">
@@ -911,8 +933,12 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
@@ -929,8 +955,9 @@
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
@@ -947,7 +974,9 @@
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -962,6 +991,9 @@
       <c r="E15" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
@@ -973,6 +1005,9 @@
       <c r="E16" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G16" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1">
       <c r="A17" s="1" t="s">
@@ -984,6 +1019,9 @@
       <c r="E17" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G17" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="18" spans="1:10" s="7" customFormat="1" ht="15.75" thickBot="1">
       <c r="A18" s="5" t="s">
@@ -998,8 +1036,12 @@
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
@@ -1013,6 +1055,9 @@
       <c r="E19" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G19" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1">
       <c r="A20" s="1" t="s">
@@ -1024,13 +1069,16 @@
       <c r="E20" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G20" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="21" spans="1:10" s="7" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A21" s="5" t="s">
-        <v>53</v>
+      <c r="A21" s="15" t="s">
+        <v>79</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6" t="s">
@@ -1038,20 +1086,25 @@
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="G21" s="14" t="s">
+        <v>77</v>
+      </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="7" customFormat="1" ht="15.75" thickBot="1">
@@ -1067,7 +1120,9 @@
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
@@ -1085,7 +1140,9 @@
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
+      <c r="G24" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
@@ -1103,17 +1160,19 @@
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
+      <c r="G25" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10" s="7" customFormat="1" ht="15.75" thickBot="1">
       <c r="A26" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6" t="s">
@@ -1121,39 +1180,47 @@
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
+      <c r="G26" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G27" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1">
       <c r="A28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="29" spans="1:10" s="7" customFormat="1" ht="15.75" thickBot="1">
       <c r="A29" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6" t="s">
@@ -1161,28 +1228,33 @@
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="G29" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1">
       <c r="A30" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G30" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="31" spans="1:10" s="7" customFormat="1" ht="15.75" thickBot="1">
       <c r="A31" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6" t="s">
@@ -1190,17 +1262,19 @@
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
+      <c r="G31" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="A32" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
@@ -1208,17 +1282,19 @@
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
+      <c r="G32" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
     <row r="33" spans="1:10" s="7" customFormat="1" ht="15.75" thickBot="1">
       <c r="A33" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
@@ -1226,7 +1302,9 @@
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
+      <c r="G33" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>

</xml_diff>